<commit_message>
Compilation de données et moyennes
</commit_message>
<xml_diff>
--- a/tp1/results/mean/conv.xlsx
+++ b/tp1/results/mean/conv.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D8B88B1E-78ED-4BE5-A0BD-EE74C4AD9034}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +19,43 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>serie2</t>
+  </si>
+  <si>
+    <t>serie1</t>
+  </si>
+  <si>
+    <t>serie3</t>
+  </si>
+  <si>
+    <t>serie4</t>
+  </si>
+  <si>
+    <t>serie5</t>
+  </si>
+  <si>
+    <t>serie6</t>
+  </si>
+  <si>
+    <t>exec2</t>
+  </si>
+  <si>
+    <t>moy1</t>
+  </si>
+  <si>
+    <t>myo2</t>
+  </si>
+  <si>
+    <t>exec1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -29,12 +65,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +91,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +374,517 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="8" max="8" width="10.15625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>9.9825859069824197E-4</v>
+      </c>
+      <c r="D2">
+        <v>1.67088508605957E-2</v>
+      </c>
+      <c r="E2">
+        <v>8.4077596664428697E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.781338691711425</v>
+      </c>
+      <c r="G2">
+        <v>6.3405261039733798</v>
+      </c>
+      <c r="H2">
+        <v>53.237371206283498</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3">
+        <v>5.3865909576415998E-3</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>9.8908424377441406E-2</v>
+      </c>
+      <c r="F3">
+        <v>0.77877593040466297</v>
+      </c>
+      <c r="G3">
+        <v>6.6385915279388401</v>
+      </c>
+      <c r="H3">
+        <v>53.603450059890697</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4">
+        <v>1.5627384185790998E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.9754333496093707E-4</v>
+      </c>
+      <c r="E4">
+        <v>9.9006175994873005E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.76796746253967196</v>
+      </c>
+      <c r="G4">
+        <v>6.4727728366851798</v>
+      </c>
+      <c r="H4">
+        <v>54.355583906173699</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1.48470401763916E-2</v>
+      </c>
+      <c r="E5">
+        <v>8.6436986923217704E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.77774405479431097</v>
+      </c>
+      <c r="G5">
+        <v>6.3571624755859304</v>
+      </c>
+      <c r="H5">
+        <v>82.731419086456299</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6">
+        <v>1.69494152069091E-2</v>
+      </c>
+      <c r="D6">
+        <v>9.9802017211913997E-4</v>
+      </c>
+      <c r="E6">
+        <v>0.129592180252075</v>
+      </c>
+      <c r="F6">
+        <v>0.73794460296630804</v>
+      </c>
+      <c r="G6">
+        <v>6.3237974643707204</v>
+      </c>
+      <c r="H6">
+        <v>107.33939647674499</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1.6985416412353498E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.10768437385559</v>
+      </c>
+      <c r="F7">
+        <v>0.78493189811706499</v>
+      </c>
+      <c r="G7">
+        <v>6.2895689010620099</v>
+      </c>
+      <c r="H7">
+        <v>100.500041246414</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1.6902685165405201E-2</v>
+      </c>
+      <c r="E8">
+        <v>9.3825817108154297E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.74472784996032704</v>
+      </c>
+      <c r="G8">
+        <v>6.4802944660186697</v>
+      </c>
+      <c r="H8">
+        <v>114.286639213562</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9">
+        <v>1.7528057098388599E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.6871690750122001E-2</v>
+      </c>
+      <c r="E9">
+        <v>8.9656829833984306E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.78399753570556596</v>
+      </c>
+      <c r="G9">
+        <v>6.3395922183990399</v>
+      </c>
+      <c r="H9">
+        <v>99.787257432937594</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>9.9611282348632791E-4</v>
+      </c>
+      <c r="E10">
+        <v>8.2889556884765597E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.75903582572937001</v>
+      </c>
+      <c r="G10">
+        <v>6.2895529270172101</v>
+      </c>
+      <c r="H10">
+        <v>97.033795118331895</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1.6944885253906201E-2</v>
+      </c>
+      <c r="E11">
+        <v>8.8174819946288993E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.76918148994445801</v>
+      </c>
+      <c r="G11">
+        <v>6.3396720886230398</v>
+      </c>
+      <c r="H11">
+        <v>113.780648946762</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1.55930519104003E-2</v>
+      </c>
+      <c r="E12" s="1">
+        <v>6.2522888183593694E-2</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.50166630744934004</v>
+      </c>
+      <c r="G12" s="1">
+        <v>5.9723203182220397</v>
+      </c>
+      <c r="H12" s="1">
+        <v>57.456727743148797</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>6.2510490417480399E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.48661088943481401</v>
+      </c>
+      <c r="G13">
+        <v>4.2692267894744802</v>
+      </c>
+      <c r="H13">
+        <v>46.231617212295497</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>7.9813003540038993E-3</v>
+      </c>
+      <c r="E14">
+        <v>6.2512159347534096E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.48424339294433499</v>
+      </c>
+      <c r="G14">
+        <v>4.5034873485565097</v>
+      </c>
+      <c r="H14">
+        <v>39.344277143478301</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>6.2514543533325195E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.76791119575500399</v>
+      </c>
+      <c r="G15">
+        <v>6.3417985439300502</v>
+      </c>
+      <c r="H15">
+        <v>37.723739147186201</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>8.9776515960693307E-3</v>
+      </c>
+      <c r="E16">
+        <v>7.8104972839355399E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.68540692329406705</v>
+      </c>
+      <c r="G16">
+        <v>4.2724974155425999</v>
+      </c>
+      <c r="H16">
+        <v>37.204257011413503</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1.09713077545166E-2</v>
+      </c>
+      <c r="E17">
+        <v>6.2479257583618102E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.52848339080810502</v>
+      </c>
+      <c r="G17">
+        <v>4.0210154056549001</v>
+      </c>
+      <c r="H17">
+        <v>39.864872217178302</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>6.2514066696166895E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.51206016540527299</v>
+      </c>
+      <c r="G18">
+        <v>4.5202367305755597</v>
+      </c>
+      <c r="H18">
+        <v>37.584059715270897</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>5.7547807693481397E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.51436090469360296</v>
+      </c>
+      <c r="G19">
+        <v>4.3364102840423504</v>
+      </c>
+      <c r="H19">
+        <v>39.128988027572603</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>6.2485218048095703E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.57525682449340798</v>
+      </c>
+      <c r="G20">
+        <v>3.95184898376464</v>
+      </c>
+      <c r="H20">
+        <v>39.734504699707003</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1.55947208404541E-2</v>
+      </c>
+      <c r="E21">
+        <v>6.2482357025146401E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.589849233627319</v>
+      </c>
+      <c r="G21">
+        <v>4.9964444637298504</v>
+      </c>
+      <c r="H21">
+        <v>46.1460795402526</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <f>AVERAGE(C2:C11)</f>
+        <v>5.6489706039428546E-3</v>
+      </c>
+      <c r="D24">
+        <f>AVERAGE(D2:D11)</f>
+        <v>1.0225224494934061E-2</v>
+      </c>
+      <c r="E24">
+        <f>AVERAGE(E2:E11)</f>
+        <v>9.6025276184081895E-2</v>
+      </c>
+      <c r="F24">
+        <f>AVERAGE(F2:F11)</f>
+        <v>0.76856453418731652</v>
+      </c>
+      <c r="G24">
+        <f>AVERAGE(G2:G11)</f>
+        <v>6.3871531009674021</v>
+      </c>
+      <c r="H24">
+        <f>AVERAGE(H2:H11)</f>
+        <v>87.665560269355666</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <f>AVERAGE(C12:C21)</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f>AVERAGE(D12:D21)</f>
+        <v>5.9118032455444235E-3</v>
+      </c>
+      <c r="E25">
+        <f>AVERAGE(E12:E21)</f>
+        <v>6.3567376136779735E-2</v>
+      </c>
+      <c r="F25">
+        <f>AVERAGE(F12:F21)</f>
+        <v>0.56458492279052686</v>
+      </c>
+      <c r="G25">
+        <f>AVERAGE(G12:G21)</f>
+        <v>4.718528628349298</v>
+      </c>
+      <c r="H25">
+        <f>AVERAGE(H12:H21)</f>
+        <v>42.041912245750368</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction des graphiques selon new compréhension taille exemplaire
x = 2^N
</commit_message>
<xml_diff>
--- a/tp1/results/mean/conv.xlsx
+++ b/tp1/results/mean/conv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp1\results\mean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6BC9F848-C137-460E-8B9E-DE6D20CDD14D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38752AE8-5613-44C9-82E5-0374474E4177}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16458" windowHeight="5106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="5109" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insertion" sheetId="1" r:id="rId1"/>
@@ -726,7 +726,7 @@
                     </a:pPr>
                     <a:r>
                       <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                      <a:t>f(x) = 1,4353x - 20,11</a:t>
+                      <a:t>f(x) = 2,8706x - 20,11</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US" sz="1400"/>
                   </a:p>
@@ -769,22 +769,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>8</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>18</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,7 +838,7 @@
         <c:axId val="1087317759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="6"/>
+          <c:min val="3"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -877,7 +877,23 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Taille</a:t>
+                  <a:t>Taille de l'exemplaire (log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="-25000"/>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> 2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -979,13 +995,27 @@
               <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
-                <a:pPr>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
+                      <a:sysClr val="windowText" lastClr="000000">
                         <a:lumMod val="65000"/>
                         <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      </a:sysClr>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -993,9 +1023,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Temps</a:t>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Temps (log</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="-25000">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>2</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>y)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-CA" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1011,13 +1058,27 @@
             <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
-              <a:pPr>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
+                    <a:sysClr val="windowText" lastClr="000000">
                       <a:lumMod val="65000"/>
                       <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    </a:sysClr>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -2010,102 +2071,102 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1">
-        <v>256</v>
+        <v>16</v>
       </c>
       <c r="B1">
         <v>5.6489706039428546E-3</v>
       </c>
       <c r="E1">
         <f>LOG(A1,2)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F1">
         <f>LOG(B1,2)</f>
         <v>-7.4677962914513873</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>1024</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>1.0225224494934061E-2</v>
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E6" si="0">LOG(A2,2)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2">
         <f>LOG(B2,2)</f>
         <v>-6.6117236718719861</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>4096</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>9.6025276184081895E-2</v>
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F6" si="1">LOG(B3,2)</f>
         <v>-3.3804419815902946</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>16384</v>
+        <v>128</v>
       </c>
       <c r="B4">
         <v>0.76856453418731652</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
         <v>-0.37976169086839329</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>65536</v>
+        <v>256</v>
       </c>
       <c r="B5">
         <v>6.3871531009674021</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
         <v>2.6751730325309602</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>262144</v>
+        <v>512</v>
       </c>
       <c r="B6">
         <v>87.665560269355666</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Mise en forme des données pour exécuter scripts
</commit_message>
<xml_diff>
--- a/tp1/results/mean/conv.xlsx
+++ b/tp1/results/mean/conv.xlsx
@@ -8,15 +8,74 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp1\results\mean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{38752AE8-5613-44C9-82E5-0374474E4177}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1ED6BB5-28DA-40F9-99B0-B0D7183EC80D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16457" windowHeight="5109" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16458" windowHeight="5112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="insertion" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+  <si>
+    <t>pour test rapport</t>
+  </si>
+  <si>
+    <t>x (2^N)</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>conv</t>
+  </si>
+  <si>
+    <t>f(x) = n^3</t>
+  </si>
+  <si>
+    <t>y/f(x)</t>
+  </si>
+  <si>
+    <t>pour test constantes</t>
+  </si>
+  <si>
+    <t>x y/f(x)</t>
+  </si>
+  <si>
+    <t>16.0 1.37914321385324e-06</t>
+  </si>
+  <si>
+    <t>32.0 3,12049087369814e-07</t>
+  </si>
+  <si>
+    <t>64.0 3.66307358490303e-07</t>
+  </si>
+  <si>
+    <t>128.0 3.66480128377589e-07</t>
+  </si>
+  <si>
+    <t>256.0 3.80703991709197e-07</t>
+  </si>
+  <si>
+    <t>512.0 6.53159322361318e-07</t>
+  </si>
+  <si>
+    <t>espace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.0 </t>
+  </si>
+  <si>
+    <t>f(x) x^3</t>
+  </si>
+  <si>
+    <t>f(x) y</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -157,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,6 +394,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -498,8 +563,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2069,15 +2136,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.84375" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="10" max="10" width="12.62890625" customWidth="1"/>
+    <col min="12" max="12" width="11.578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1">
         <v>16</v>
       </c>
@@ -2092,8 +2163,31 @@
         <f>LOG(B1,2)</f>
         <v>-7.4677962914513873</v>
       </c>
+      <c r="J1">
+        <f>A1^3</f>
+        <v>4096</v>
+      </c>
+      <c r="K1">
+        <f>B1</f>
+        <v>5.6489706039428546E-3</v>
+      </c>
+      <c r="L1">
+        <f>K1/J1</f>
+        <v>1.379143213853236E-6</v>
+      </c>
+      <c r="M1" t="str">
+        <f>_xlfn.CONCAT(A1,$H$7,L1)</f>
+        <v>16.0 1,37914321385324E-06</v>
+      </c>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="str">
+        <f>_xlfn.CONCAT(J1,$H$7,B1)</f>
+        <v>4096.0 0,00564897060394285</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>32</v>
       </c>
@@ -2108,8 +2202,31 @@
         <f>LOG(B2,2)</f>
         <v>-6.6117236718719861</v>
       </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J6" si="1">A2^3</f>
+        <v>32768</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ref="K2:K6" si="2">B2</f>
+        <v>1.0225224494934061E-2</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L6" si="3">K2/J2</f>
+        <v>3.1204908736981386E-7</v>
+      </c>
+      <c r="M2" t="str">
+        <f t="shared" ref="M2:M6" si="4">_xlfn.CONCAT(A2,$H$7,L2)</f>
+        <v>32.0 3,12049087369814E-07</v>
+      </c>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T2" t="str">
+        <f t="shared" ref="T2:T6" si="5">_xlfn.CONCAT(J2,$H$7,B2)</f>
+        <v>32768.0 0,0102252244949341</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <v>64</v>
       </c>
@@ -2121,11 +2238,34 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F6" si="1">LOG(B3,2)</f>
+        <f t="shared" ref="F3:F6" si="6">LOG(B3,2)</f>
         <v>-3.3804419815902946</v>
       </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>262144</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="2"/>
+        <v>9.6025276184081895E-2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="3"/>
+        <v>3.6630735849030264E-7</v>
+      </c>
+      <c r="M3" t="str">
+        <f t="shared" si="4"/>
+        <v>64.0 3,66307358490303E-07</v>
+      </c>
+      <c r="P3" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" t="str">
+        <f t="shared" si="5"/>
+        <v>262144.0 0,0960252761840819</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <v>128</v>
       </c>
@@ -2137,11 +2277,34 @@
         <v>7</v>
       </c>
       <c r="F4">
+        <f t="shared" si="6"/>
+        <v>-0.37976169086839329</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="1"/>
-        <v>-0.37976169086839329</v>
+        <v>2097152</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0.76856453418731652</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="3"/>
+        <v>3.6648012837758852E-7</v>
+      </c>
+      <c r="M4" t="str">
+        <f t="shared" si="4"/>
+        <v>128.0 3,66480128377589E-07</v>
+      </c>
+      <c r="P4" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" t="str">
+        <f t="shared" si="5"/>
+        <v>2097152.0 0,768564534187317</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <v>256</v>
       </c>
@@ -2153,11 +2316,34 @@
         <v>8</v>
       </c>
       <c r="F5">
+        <f t="shared" si="6"/>
+        <v>2.6751730325309602</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="1"/>
-        <v>2.6751730325309602</v>
+        <v>16777216</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>6.3871531009674021</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="3"/>
+        <v>3.8070399170919669E-7</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" si="4"/>
+        <v>256.0 3,80703991709197E-07</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="T5" t="str">
+        <f t="shared" si="5"/>
+        <v>16777216.0 6,3871531009674</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>512</v>
       </c>
@@ -2169,8 +2355,84 @@
         <v>9</v>
       </c>
       <c r="F6">
+        <f t="shared" si="6"/>
+        <v>6.4539382809211121</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
-        <v>6.4539382809211121</v>
+        <v>134217728</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>87.665560269355666</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="3"/>
+        <v>6.5315932236131777E-7</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" si="4"/>
+        <v>512.0 6,53159322361318E-07</v>
+      </c>
+      <c r="P6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T6" t="str">
+        <f t="shared" si="5"/>
+        <v>134217728.0 87,6655602693557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>7</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T7" t="s">
+        <v>17</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise en forme csv pour test rapp et cte
</commit_message>
<xml_diff>
--- a/tp1/results/mean/conv.xlsx
+++ b/tp1/results/mean/conv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp1\results\mean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A1ED6BB5-28DA-40F9-99B0-B0D7183EC80D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{437FAE86-2D50-4C34-9EB4-74A0E994C5CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16458" windowHeight="5112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>pour test rapport</t>
   </si>
@@ -74,6 +74,36 @@
   </si>
   <si>
     <t>f(x) y</t>
+  </si>
+  <si>
+    <t>logx</t>
+  </si>
+  <si>
+    <t>logy</t>
+  </si>
+  <si>
+    <t>rapport</t>
+  </si>
+  <si>
+    <t>constatnes</t>
+  </si>
+  <si>
+    <t>4096.0 0.00564897060394285</t>
+  </si>
+  <si>
+    <t>32768.0 0.0102252244949341</t>
+  </si>
+  <si>
+    <t>262144.0 0.0960252761840819</t>
+  </si>
+  <si>
+    <t>2097152.0 0.768564534187317</t>
+  </si>
+  <si>
+    <t>16777216.0 6.3871531009674</t>
+  </si>
+  <si>
+    <t>134217728.0 87.6655602693557</t>
   </si>
 </sst>
 </file>
@@ -2138,8 +2168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2186,6 +2216,9 @@
         <f>_xlfn.CONCAT(J1,$H$7,B1)</f>
         <v>4096.0 0,00564897060394285</v>
       </c>
+      <c r="X1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
@@ -2225,6 +2258,9 @@
         <f t="shared" ref="T2:T6" si="5">_xlfn.CONCAT(J2,$H$7,B2)</f>
         <v>32768.0 0,0102252244949341</v>
       </c>
+      <c r="X2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
@@ -2264,6 +2300,9 @@
         <f t="shared" si="5"/>
         <v>262144.0 0,0960252761840819</v>
       </c>
+      <c r="X3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
@@ -2303,6 +2342,9 @@
         <f t="shared" si="5"/>
         <v>2097152.0 0,768564534187317</v>
       </c>
+      <c r="X4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
@@ -2342,6 +2384,9 @@
         <f t="shared" si="5"/>
         <v>16777216.0 6,3871531009674</v>
       </c>
+      <c r="X5" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -2381,6 +2426,9 @@
         <f t="shared" si="5"/>
         <v>134217728.0 87,6655602693557</v>
       </c>
+      <c r="X6" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
@@ -2389,6 +2437,12 @@
       <c r="B7" t="s">
         <v>2</v>
       </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>19</v>
+      </c>
       <c r="H7" t="s">
         <v>15</v>
       </c>
@@ -2426,8 +2480,14 @@
       <c r="J8" t="s">
         <v>0</v>
       </c>
+      <c r="P8" t="s">
+        <v>20</v>
+      </c>
       <c r="T8" t="s">
         <v>6</v>
+      </c>
+      <c r="X8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Rapport fini, hack excel pour obtenir le coefficient de regression linaire
</commit_message>
<xml_diff>
--- a/tp1/results/mean/conv.xlsx
+++ b/tp1/results/mean/conv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp1\results\mean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{437FAE86-2D50-4C34-9EB4-74A0E994C5CE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{71F38271-7330-4DFD-9E90-7A2B25D20B35}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16458" windowHeight="5112" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1272,7 +1272,476 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="0"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.4206474190726159E-2"/>
+                  <c:y val="-0.17827354913969087"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="fr-CA" sz="800">
+                        <a:solidFill>
+                          <a:sysClr val="windowText" lastClr="000000"/>
+                        </a:solidFill>
+                        <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                        <a:ea typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+                        <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+                      </a:rPr>
+                      <a:t>R² = 0,9974</a:t>
+                    </a:r>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="fr-FR"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>insertion!$J$1:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32768</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>262144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2097152</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16777216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>134217728</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>insertion!$K$1:$K$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.6489706039428546E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0225224494934061E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.6025276184081895E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.76856453418731652</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3871531009674021</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87.665560269355666</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BEC9-4540-A6B2-637D4AA7C034}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="404958448"/>
+        <c:axId val="404958776"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="404958448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404958776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="404958776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="404958448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1828,6 +2297,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1861,6 +2846,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>158115</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>417195</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8D565F1-6FF9-4965-9CF7-8B5CF5DA9536}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2168,8 +3189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>